<commit_message>
optimization of the copying process when receiving data [--stable]
</commit_message>
<xml_diff>
--- a/necessary/Дневник.xlsx
+++ b/necessary/Дневник.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MRX\Downloads\Диплом\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MRX\Downloads\Диплом\Pipeline\necessary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4F8800-42E2-4ECA-B1C2-120EBF40C7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E081D5-35BD-40F5-95DE-3D77E386CAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F43ECF24-9B2C-41F7-931C-C61107D1C769}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Дата</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Установка библиотеки для многопоточной очереди типа mpmc из библиотеки cds, а также ее интеграция в проект</t>
+  </si>
+  <si>
+    <t>15 марта</t>
+  </si>
+  <si>
+    <t>Поиск инструмента для отслеживания утечек памяти, а также написание про него текста в теории вкр, оптимизация копирований при приеме данных</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +665,12 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>

</xml_diff>

<commit_message>
Optimize data copying between stages and improve thread for monitoring [--stable]
</commit_message>
<xml_diff>
--- a/necessary/Дневник.xlsx
+++ b/necessary/Дневник.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MRX\Downloads\Диплом\Pipeline\necessary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E081D5-35BD-40F5-95DE-3D77E386CAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2C41FF-93E4-4557-98E4-4E3A84FC494C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F43ECF24-9B2C-41F7-931C-C61107D1C769}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{F43ECF24-9B2C-41F7-931C-C61107D1C769}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Дата</t>
   </si>
@@ -139,6 +139,24 @@
   </si>
   <si>
     <t>Поиск инструмента для отслеживания утечек памяти, а также написание про него текста в теории вкр, оптимизация копирований при приеме данных</t>
+  </si>
+  <si>
+    <t>16  марта</t>
+  </si>
+  <si>
+    <t>Написание потока для мониторинга работы стадий конвейера</t>
+  </si>
+  <si>
+    <t>17 марта</t>
+  </si>
+  <si>
+    <t>Написание теорической части вкр, оптимизация передачи данных между стадиями конвейера (оптимизация копирования)</t>
+  </si>
+  <si>
+    <t>18 марта</t>
+  </si>
+  <si>
+    <t>Усовершенствование потока для мониторинга конвейера: добавлено снятие замеров времени, которое стадии затрачивают на выполнение функтора</t>
   </si>
 </sst>
 </file>
@@ -502,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB2592C-4FA5-4CA6-99FF-E36C50D0F62A}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,13 +691,28 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>

</xml_diff>

<commit_message>
ready benchmark for Lockfree queues [--unstable]
</commit_message>
<xml_diff>
--- a/necessary/Дневник.xlsx
+++ b/necessary/Дневник.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MRX\Downloads\Диплом\Pipeline\necessary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2C41FF-93E4-4557-98E4-4E3A84FC494C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A4C46D-83A0-45B7-AF04-B1345033DDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{F43ECF24-9B2C-41F7-931C-C61107D1C769}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F43ECF24-9B2C-41F7-931C-C61107D1C769}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Дата</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>Усовершенствование потока для мониторинга конвейера: добавлено снятие замеров времени, которое стадии затрачивают на выполнение функтора</t>
+  </si>
+  <si>
+    <t>19 марта</t>
+  </si>
+  <si>
+    <t>Правка теоритической части текста в черновике вкр. Создание проекта для проведения бенчмарков различных библиотек, а также написание самих бенчмарков</t>
   </si>
 </sst>
 </file>
@@ -521,13 +527,13 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="148.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="153.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -715,8 +721,12 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>

</xml_diff>

<commit_message>
Benchmarks are ready. (writing a benchmark testStageDataType) [--stable]
</commit_message>
<xml_diff>
--- a/necessary/Дневник.xlsx
+++ b/necessary/Дневник.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MRX\Downloads\Диплом\Pipeline\necessary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A4C46D-83A0-45B7-AF04-B1345033DDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4FA81F-C642-4B09-BDD8-7BD5F74E8F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F43ECF24-9B2C-41F7-931C-C61107D1C769}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Дата</t>
   </si>
@@ -162,7 +162,13 @@
     <t>19 марта</t>
   </si>
   <si>
-    <t>Правка теоритической части текста в черновике вкр. Создание проекта для проведения бенчмарков различных библиотек, а также написание самих бенчмарков</t>
+    <t>20 марта</t>
+  </si>
+  <si>
+    <t>Правка теоритической части текста в черновике вкр. Создание проекта для проведения бенчмарков различных библиотек, а также написание бенчмарка для тестирования скорости коннекторов (очередей) (бенчмарк testLockfreeQueues)</t>
+  </si>
+  <si>
+    <t>Написание бенчмарка для тестирования структур данных, в которых хранятся данные, которые обрабатываются стадиями конвейера (бенчмарк testStageDataType)</t>
   </si>
 </sst>
 </file>
@@ -526,14 +532,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB2592C-4FA5-4CA6-99FF-E36C50D0F62A}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="153.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="226.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -725,12 +731,16 @@
         <v>41</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>

</xml_diff>

<commit_message>
readme file for benchmark project. Update necessary files. [--stable]
</commit_message>
<xml_diff>
--- a/necessary/Дневник.xlsx
+++ b/necessary/Дневник.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MRX\Downloads\Диплом\Pipeline\necessary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F7C061-B7AD-4B30-BF88-9AF2E166106C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89507D75-9C0B-417E-A166-53504FD06906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F43ECF24-9B2C-41F7-931C-C61107D1C769}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Дата</t>
   </si>
@@ -187,6 +187,18 @@
   </si>
   <si>
     <t>Написание Менеджера для десериализации данных (для cv::Mat и для xTensor). Фикс файла Cmakelists.txt для проекта с бенчмарками</t>
+  </si>
+  <si>
+    <t>24 марта</t>
+  </si>
+  <si>
+    <t>25 марта</t>
+  </si>
+  <si>
+    <t>Окончательный рефакторинг проекта бенчмаров и оформление проекта</t>
+  </si>
+  <si>
+    <t>Написание скрипта на python для построения графика по данным результатов работы бенчмарка</t>
   </si>
 </sst>
 </file>
@@ -551,7 +563,7 @@
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,10 +797,20 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>

</xml_diff>

<commit_message>
writing a generator for sending 4k frames from video. Minor fixes [--stable]
</commit_message>
<xml_diff>
--- a/necessary/Дневник.xlsx
+++ b/necessary/Дневник.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MRX\Downloads\Диплом\Pipeline\necessary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89507D75-9C0B-417E-A166-53504FD06906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E274AE11-B7B5-45A7-8BD2-CE58FEF9C848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F43ECF24-9B2C-41F7-931C-C61107D1C769}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Дата</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>Написание скрипта на python для построения графика по данным результатов работы бенчмарка</t>
+  </si>
+  <si>
+    <t>26 марта</t>
+  </si>
+  <si>
+    <t>Декомпозиция кода (написание NetworkReceiveManager и вынесение структуры Measurements)</t>
+  </si>
+  <si>
+    <t>27 марта</t>
+  </si>
+  <si>
+    <t>Написание генератора для выдачи 4к изображений из видео и адаптация и мелкие фиксы</t>
   </si>
 </sst>
 </file>
@@ -563,7 +575,7 @@
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,10 +825,20 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>

</xml_diff>

<commit_message>
update CMakeLists.txt and necessary files [--stable]
</commit_message>
<xml_diff>
--- a/necessary/Дневник.xlsx
+++ b/necessary/Дневник.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MRX\Downloads\Диплом\Pipeline\necessary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E274AE11-B7B5-45A7-8BD2-CE58FEF9C848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D008E3AE-7A52-4EF2-A99A-B100866B97D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F43ECF24-9B2C-41F7-931C-C61107D1C769}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Дата</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>Написание генератора для выдачи 4к изображений из видео и адаптация и мелкие фиксы</t>
+  </si>
+  <si>
+    <t>28 марта</t>
+  </si>
+  <si>
+    <t>Интеграция функций cv::Mat в проект и тестирование работы конвейера</t>
   </si>
 </sst>
 </file>
@@ -575,7 +581,7 @@
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +847,12 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>

</xml_diff>